<commit_message>
Printing page fault data
</commit_message>
<xml_diff>
--- a/Yeezus/resources/template.xlsx
+++ b/Yeezus/resources/template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Mark Zeagler\Documents\GitHub\CS3502_Group_Project\Yeezus\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E367268B-E1E4-496B-A811-FDBEFE38B894}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Process ID:</t>
   </si>
@@ -63,12 +64,18 @@
   </si>
   <si>
     <t>% of Cache</t>
+  </si>
+  <si>
+    <t># of Page Faults:</t>
+  </si>
+  <si>
+    <t>Average page fault servicing time (ns):</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,9 +113,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,32 +156,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Process_Table" displayName="Process_Table" ref="A1:I32" totalsRowCount="1">
-  <autoFilter ref="A1:I31"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Process ID:" totalsRowLabel="Average" totalsRowDxfId="0"/>
-    <tableColumn id="2" name="Wait Time (ms):" totalsRowFunction="custom">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Process_Table" displayName="Process_Table" ref="A1:K32" totalsRowCount="1">
+  <autoFilter ref="A1:K31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Process ID:" totalsRowLabel="Average" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Wait Time (ms):" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Process_Table[Wait Time (ms):])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Run Time (ms):" totalsRowFunction="custom">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Run Time (ms):" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Process_Table[Run Time (ms):])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Completion Time (ms):" totalsRowFunction="custom">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Completion Time (ms):" totalsRowFunction="custom">
       <calculatedColumnFormula>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</calculatedColumnFormula>
       <totalsRowFormula>AVERAGE(Process_Table[Completion Time (ms):])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Execution Count:" totalsRowFunction="custom">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Execution Count:" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Process_Table[Execution Count:])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="I/O Count:" totalsRowFunction="custom">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="I/O Count:" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Process_Table[I/O Count:])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="CPU"/>
-    <tableColumn id="9" name="% of Cache" totalsRowFunction="custom">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="CPU"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="% of Cache" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Process_Table[% of Cache])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="% of RAM" totalsRowFunction="custom">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="% of RAM" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Process_Table[% of RAM])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{6CC54309-D32B-4098-A6C1-0863CC381CF5}" name="# of Page Faults:" totalsRowFunction="custom">
+      <totalsRowFormula>AVERAGE(Process_Table['# of Page Faults:])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{47975D68-1810-46F1-9DD0-4B807EF02AE9}" name="Average page fault servicing time (ns):" totalsRowFunction="custom">
+      <totalsRowFormula>AVERAGE(Process_Table[Average page fault servicing time (ns):])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -179,14 +195,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="CPU_Table" displayName="CPU_Table" ref="K1:M3" insertRow="1" totalsRowCount="1">
-  <autoFilter ref="K1:M2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="CPU_Table" displayName="CPU_Table" ref="M1:O3" insertRow="1" totalsRowCount="1">
+  <autoFilter ref="M1:O2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="CPU ID:" totalsRowLabel="Average"/>
-    <tableColumn id="2" name="Busy Time (ms):" totalsRowFunction="custom">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CPU ID:" totalsRowLabel="Average"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Busy Time (ms):" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(CPU_Table[Busy Time (ms):])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Idle Time (ms):" totalsRowFunction="custom">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Idle Time (ms):" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(CPU_Table[Idle Time (ms):])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -490,11 +506,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,13 +523,15 @@
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,208 +559,214 @@
       <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D2">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D3">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>4</v>
       </c>
-      <c r="L3" t="e">
+      <c r="N3" t="e">
         <f>AVERAGE(CPU_Table[Busy Time (ms):])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M3" t="e">
+      <c r="O3" t="e">
         <f>AVERAGE(CPU_Table[Idle Time (ms):])</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D5">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D11">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D13">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D18">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D19">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D20">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D21">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D22">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D23">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D24">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D25">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D26">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D28">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31">
         <f>Process_Table[Run Time (ms):]+Process_Table[Wait Time (ms):]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -772,6 +796,14 @@
       </c>
       <c r="I32" t="e">
         <f>AVERAGE(Process_Table[% of RAM])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J32" t="e">
+        <f>AVERAGE(Process_Table['# of Page Faults:])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K32" t="e">
+        <f>AVERAGE(Process_Table[Average page fault servicing time (ns):])</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>